<commit_message>
Updated Test Data sheet for TC-54238
</commit_message>
<xml_diff>
--- a/Test Data/TC_54238_Verify_When_User_Select_FOM_MPM800_ANN880_It_Should_Get_Added_To_Shopping_List.xlsx
+++ b/Test Data/TC_54238_Verify_When_User_Select_FOM_MPM800_ANN880_It_Should_Get_Added_To_Shopping_List.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E717B4-E1DA-4FCE-8606-66C1598DD92F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,9 +207,6 @@
     <t>MPM800</t>
   </si>
   <si>
-    <t>FOM800 Fibre Optic Modules</t>
-  </si>
-  <si>
     <t>FOM Shopping List</t>
   </si>
   <si>
@@ -239,12 +235,15 @@
   </si>
   <si>
     <t>To verify shopping list on selecting FOM and MPM devices</t>
+  </si>
+  <si>
+    <t>FOM800 Fibre Optic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,11 +674,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +708,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>0</v>
@@ -721,7 +720,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8" t="s">
@@ -733,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="8" t="s">
@@ -784,31 +783,31 @@
         <v>55</v>
       </c>
       <c r="K7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="N7" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="N7" s="19" t="s">
+      <c r="P7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="Q7" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q7" s="19" t="s">
+      <c r="R7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="R7" s="19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -843,7 +842,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="M8" s="20" t="s">
         <v>57</v>
@@ -874,7 +873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCE740E-15F1-4A53-8BB2-F229CF1FB15E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>